<commit_message>
Updated Adaptive shortest path
</commit_message>
<xml_diff>
--- a/StochasticShortestPath_Static/Parameters.xlsx
+++ b/StochasticShortestPath_Static/Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnascime/Dropbox/PythonProjects/ORF411/github_private/seqdecisionlib_ShortestPath_Static/Stochastic_Shortest_Path_Static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade0001\Documents\01 - Vorlesungen\Stochastische Optimierungsprobleme\stochastic-optimization\StochasticShortestPath_Static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ADB17F-37F4-DE4A-833C-20B1D8953E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F7CAED-AD73-4A85-A6DE-2CC784C5E70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="680" windowWidth="19620" windowHeight="10160" activeTab="1" xr2:uid="{0DB32CC8-A0F8-4A1F-8469-0451A56A93A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0DB32CC8-A0F8-4A1F-8469-0451A56A93A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>probEdge</t>
   </si>
   <si>
-    <t>1 .5 .2 .1</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Use sheet </t>
     </r>
@@ -229,6 +226,9 @@
       </rPr>
       <t xml:space="preserve"> inside "StaticModelAdaptive.py"</t>
     </r>
+  </si>
+  <si>
+    <t>1 0.5 0.2 0.01</t>
   </si>
 </sst>
 </file>
@@ -603,42 +603,42 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.1640625" customWidth="1"/>
+    <col min="1" max="1" width="83.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -651,16 +651,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -668,23 +668,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -692,7 +692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -700,15 +700,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -716,12 +716,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>